<commit_message>
Completion of Form 16 2017-18'
</commit_message>
<xml_diff>
--- a/savings.xlsx
+++ b/savings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="220">
   <si>
     <t>NAME</t>
   </si>
@@ -673,6 +673,9 @@
   </si>
   <si>
     <t>SC</t>
+  </si>
+  <si>
+    <t>ROP</t>
   </si>
 </sst>
 </file>
@@ -2372,10 +2375,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S94"/>
+  <dimension ref="A1:T94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2396,7 +2399,7 @@
     <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1">
+    <row r="1" spans="1:20" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2454,8 +2457,11 @@
       <c r="S1" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -2510,8 +2516,11 @@
       <c r="S2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -2566,8 +2575,11 @@
       <c r="S3">
         <v>359</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -2622,8 +2634,11 @@
       <c r="S4">
         <v>548</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="T4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -2678,8 +2693,11 @@
       <c r="S5">
         <v>315</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -2734,8 +2752,11 @@
       <c r="S6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
@@ -2790,8 +2811,11 @@
       <c r="S7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="T7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -2846,8 +2870,11 @@
       <c r="S8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
@@ -2902,8 +2929,11 @@
       <c r="S9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="T9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -2958,8 +2988,11 @@
       <c r="S10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
@@ -3014,8 +3047,11 @@
       <c r="S11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="T11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -3070,8 +3106,11 @@
       <c r="S12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:19">
+      <c r="T12">
+        <v>26425</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
@@ -3126,8 +3165,11 @@
       <c r="S13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="T13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -3182,8 +3224,11 @@
       <c r="S14">
         <v>354</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -3238,8 +3283,11 @@
       <c r="S15">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="T15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>44</v>
       </c>
@@ -3294,8 +3342,11 @@
       <c r="S16">
         <v>570</v>
       </c>
-    </row>
-    <row r="17" spans="1:19">
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -3350,8 +3401,11 @@
       <c r="S17">
         <v>207</v>
       </c>
-    </row>
-    <row r="18" spans="1:19">
+      <c r="T17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" s="5" t="s">
         <v>48</v>
       </c>
@@ -3406,8 +3460,11 @@
       <c r="S18">
         <v>227</v>
       </c>
-    </row>
-    <row r="19" spans="1:19">
+      <c r="T18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>50</v>
       </c>
@@ -3462,8 +3519,11 @@
       <c r="S19">
         <v>936</v>
       </c>
-    </row>
-    <row r="20" spans="1:19">
+      <c r="T19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
@@ -3518,8 +3578,11 @@
       <c r="S20">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="T20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>54</v>
       </c>
@@ -3574,8 +3637,11 @@
       <c r="S21">
         <v>279</v>
       </c>
-    </row>
-    <row r="22" spans="1:19">
+      <c r="T21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" s="5" t="s">
         <v>56</v>
       </c>
@@ -3630,8 +3696,11 @@
       <c r="S22">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:19">
+      <c r="T22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
@@ -3686,8 +3755,11 @@
       <c r="S23">
         <v>169</v>
       </c>
-    </row>
-    <row r="24" spans="1:19">
+      <c r="T23">
+        <v>30993</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24" s="5" t="s">
         <v>60</v>
       </c>
@@ -3742,8 +3814,11 @@
       <c r="S24">
         <v>52</v>
       </c>
-    </row>
-    <row r="25" spans="1:19">
+      <c r="T24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25" s="4" t="s">
         <v>62</v>
       </c>
@@ -3798,8 +3873,11 @@
       <c r="S25">
         <v>159</v>
       </c>
-    </row>
-    <row r="26" spans="1:19">
+      <c r="T25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26" s="5" t="s">
         <v>64</v>
       </c>
@@ -3854,8 +3932,11 @@
       <c r="S26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:19">
+      <c r="T26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" s="4" t="s">
         <v>66</v>
       </c>
@@ -3910,8 +3991,11 @@
       <c r="S27">
         <v>210</v>
       </c>
-    </row>
-    <row r="28" spans="1:19">
+      <c r="T27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28" s="5" t="s">
         <v>68</v>
       </c>
@@ -3966,8 +4050,11 @@
       <c r="S28">
         <v>270</v>
       </c>
-    </row>
-    <row r="29" spans="1:19">
+      <c r="T28">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29" s="4" t="s">
         <v>70</v>
       </c>
@@ -4022,8 +4109,11 @@
       <c r="S29">
         <v>264</v>
       </c>
-    </row>
-    <row r="30" spans="1:19">
+      <c r="T29">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" s="5" t="s">
         <v>72</v>
       </c>
@@ -4078,8 +4168,11 @@
       <c r="S30">
         <v>535</v>
       </c>
-    </row>
-    <row r="31" spans="1:19">
+      <c r="T30">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31" s="4" t="s">
         <v>74</v>
       </c>
@@ -4134,8 +4227,11 @@
       <c r="S31">
         <v>231</v>
       </c>
-    </row>
-    <row r="32" spans="1:19">
+      <c r="T31">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32" s="5" t="s">
         <v>76</v>
       </c>
@@ -4190,8 +4286,11 @@
       <c r="S32">
         <v>167</v>
       </c>
-    </row>
-    <row r="33" spans="1:19">
+      <c r="T32">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
       <c r="A33" s="4" t="s">
         <v>78</v>
       </c>
@@ -4246,8 +4345,11 @@
       <c r="S33">
         <v>349</v>
       </c>
-    </row>
-    <row r="34" spans="1:19">
+      <c r="T33">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
       <c r="A34" s="5" t="s">
         <v>80</v>
       </c>
@@ -4302,8 +4404,11 @@
       <c r="S34">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:19">
+      <c r="T34">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
       <c r="A35" s="4" t="s">
         <v>82</v>
       </c>
@@ -4358,8 +4463,11 @@
       <c r="S35">
         <v>340</v>
       </c>
-    </row>
-    <row r="36" spans="1:19">
+      <c r="T35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
       <c r="A36" s="5" t="s">
         <v>84</v>
       </c>
@@ -4414,8 +4522,11 @@
       <c r="S36">
         <v>298</v>
       </c>
-    </row>
-    <row r="37" spans="1:19">
+      <c r="T36">
+        <v>3892</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
       <c r="A37" s="4" t="s">
         <v>86</v>
       </c>
@@ -4470,8 +4581,11 @@
       <c r="S37">
         <v>473</v>
       </c>
-    </row>
-    <row r="38" spans="1:19">
+      <c r="T37">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20">
       <c r="A38" s="5" t="s">
         <v>88</v>
       </c>
@@ -4526,8 +4640,11 @@
       <c r="S38">
         <v>307</v>
       </c>
-    </row>
-    <row r="39" spans="1:19">
+      <c r="T38">
+        <v>28912</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
       <c r="A39" s="4" t="s">
         <v>90</v>
       </c>
@@ -4582,8 +4699,11 @@
       <c r="S39">
         <v>326</v>
       </c>
-    </row>
-    <row r="40" spans="1:19">
+      <c r="T39">
+        <v>3892</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
       <c r="A40" s="5" t="s">
         <v>92</v>
       </c>
@@ -4638,8 +4758,11 @@
       <c r="S40">
         <v>684</v>
       </c>
-    </row>
-    <row r="41" spans="1:19">
+      <c r="T40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
       <c r="A41" s="4" t="s">
         <v>94</v>
       </c>
@@ -4694,8 +4817,11 @@
       <c r="S41">
         <v>151</v>
       </c>
-    </row>
-    <row r="42" spans="1:19">
+      <c r="T41">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
       <c r="A42" s="5" t="s">
         <v>96</v>
       </c>
@@ -4750,8 +4876,11 @@
       <c r="S42">
         <v>74</v>
       </c>
-    </row>
-    <row r="43" spans="1:19">
+      <c r="T42">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
       <c r="A43" s="4" t="s">
         <v>98</v>
       </c>
@@ -4806,8 +4935,11 @@
       <c r="S43">
         <v>239</v>
       </c>
-    </row>
-    <row r="44" spans="1:19">
+      <c r="T43">
+        <v>17991</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
       <c r="A44" s="5" t="s">
         <v>100</v>
       </c>
@@ -4862,8 +4994,11 @@
       <c r="S44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="T44">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
       <c r="A45" s="4" t="s">
         <v>102</v>
       </c>
@@ -4918,8 +5053,11 @@
       <c r="S45">
         <v>326</v>
       </c>
-    </row>
-    <row r="46" spans="1:19">
+      <c r="T45">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
       <c r="A46" s="5" t="s">
         <v>104</v>
       </c>
@@ -4974,8 +5112,11 @@
       <c r="S46">
         <v>384</v>
       </c>
-    </row>
-    <row r="47" spans="1:19">
+      <c r="T46">
+        <v>13696</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
       <c r="A47" s="4" t="s">
         <v>106</v>
       </c>
@@ -5030,8 +5171,11 @@
       <c r="S47">
         <v>163</v>
       </c>
-    </row>
-    <row r="48" spans="1:19">
+      <c r="T47">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
       <c r="A48" s="5" t="s">
         <v>108</v>
       </c>
@@ -5086,8 +5230,11 @@
       <c r="S48">
         <v>173</v>
       </c>
-    </row>
-    <row r="49" spans="1:19">
+      <c r="T48">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
       <c r="A49" s="4" t="s">
         <v>110</v>
       </c>
@@ -5142,8 +5289,11 @@
       <c r="S49">
         <v>158</v>
       </c>
-    </row>
-    <row r="50" spans="1:19">
+      <c r="T49">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20">
       <c r="A50" s="5" t="s">
         <v>112</v>
       </c>
@@ -5198,8 +5348,11 @@
       <c r="S50">
         <v>226</v>
       </c>
-    </row>
-    <row r="51" spans="1:19">
+      <c r="T50">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51" s="4" t="s">
         <v>114</v>
       </c>
@@ -5254,8 +5407,11 @@
       <c r="S51">
         <v>290</v>
       </c>
-    </row>
-    <row r="52" spans="1:19">
+      <c r="T51">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
       <c r="A52" s="5" t="s">
         <v>116</v>
       </c>
@@ -5310,8 +5466,11 @@
       <c r="S52">
         <v>458</v>
       </c>
-    </row>
-    <row r="53" spans="1:19">
+      <c r="T52">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" s="4" t="s">
         <v>118</v>
       </c>
@@ -5366,8 +5525,11 @@
       <c r="S53">
         <v>538</v>
       </c>
-    </row>
-    <row r="54" spans="1:19">
+      <c r="T53">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20">
       <c r="A54" s="5" t="s">
         <v>120</v>
       </c>
@@ -5419,8 +5581,11 @@
       <c r="S54">
         <v>183</v>
       </c>
-    </row>
-    <row r="55" spans="1:19">
+      <c r="T54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55" s="4" t="s">
         <v>122</v>
       </c>
@@ -5475,8 +5640,11 @@
       <c r="S55">
         <v>75</v>
       </c>
-    </row>
-    <row r="56" spans="1:19">
+      <c r="T55">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56" s="5" t="s">
         <v>124</v>
       </c>
@@ -5531,8 +5699,11 @@
       <c r="S56">
         <v>350</v>
       </c>
-    </row>
-    <row r="57" spans="1:19">
+      <c r="T56">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57" s="4" t="s">
         <v>126</v>
       </c>
@@ -5587,8 +5758,11 @@
       <c r="S57">
         <v>323</v>
       </c>
-    </row>
-    <row r="58" spans="1:19">
+      <c r="T57">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20">
       <c r="A58" s="5" t="s">
         <v>128</v>
       </c>
@@ -5643,8 +5817,11 @@
       <c r="S58">
         <v>32</v>
       </c>
-    </row>
-    <row r="59" spans="1:19">
+      <c r="T58">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20">
       <c r="A59" s="4" t="s">
         <v>130</v>
       </c>
@@ -5699,8 +5876,11 @@
       <c r="S59">
         <v>231</v>
       </c>
-    </row>
-    <row r="60" spans="1:19">
+      <c r="T59">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60" s="5" t="s">
         <v>132</v>
       </c>
@@ -5755,8 +5935,11 @@
       <c r="S60">
         <v>307</v>
       </c>
-    </row>
-    <row r="61" spans="1:19">
+      <c r="T60">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61" s="4" t="s">
         <v>134</v>
       </c>
@@ -5811,8 +5994,11 @@
       <c r="S61">
         <v>184</v>
       </c>
-    </row>
-    <row r="62" spans="1:19">
+      <c r="T61">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20">
       <c r="A62" s="5" t="s">
         <v>136</v>
       </c>
@@ -5867,8 +6053,11 @@
       <c r="S62">
         <v>463</v>
       </c>
-    </row>
-    <row r="63" spans="1:19">
+      <c r="T62">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20">
       <c r="A63" s="4" t="s">
         <v>138</v>
       </c>
@@ -5923,8 +6112,11 @@
       <c r="S63">
         <v>260</v>
       </c>
-    </row>
-    <row r="64" spans="1:19">
+      <c r="T63">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
       <c r="A64" s="5" t="s">
         <v>140</v>
       </c>
@@ -5979,8 +6171,11 @@
       <c r="S64">
         <v>359</v>
       </c>
-    </row>
-    <row r="65" spans="1:19">
+      <c r="T64">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
       <c r="A65" s="4" t="s">
         <v>142</v>
       </c>
@@ -6035,8 +6230,11 @@
       <c r="S65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:19">
+      <c r="T65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66" s="5" t="s">
         <v>144</v>
       </c>
@@ -6091,8 +6289,11 @@
       <c r="S66">
         <v>439</v>
       </c>
-    </row>
-    <row r="67" spans="1:19">
+      <c r="T66">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
       <c r="A67" s="4" t="s">
         <v>146</v>
       </c>
@@ -6147,8 +6348,11 @@
       <c r="S67">
         <v>175</v>
       </c>
-    </row>
-    <row r="68" spans="1:19">
+      <c r="T67">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
       <c r="A68" s="5" t="s">
         <v>148</v>
       </c>
@@ -6203,8 +6407,11 @@
       <c r="S68">
         <v>166</v>
       </c>
-    </row>
-    <row r="69" spans="1:19">
+      <c r="T68">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69" s="4" t="s">
         <v>150</v>
       </c>
@@ -6259,8 +6466,11 @@
       <c r="S69">
         <v>375</v>
       </c>
-    </row>
-    <row r="70" spans="1:19">
+      <c r="T69">
+        <v>11092</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70" s="5" t="s">
         <v>152</v>
       </c>
@@ -6315,8 +6525,11 @@
       <c r="S70">
         <v>178</v>
       </c>
-    </row>
-    <row r="71" spans="1:19">
+      <c r="T70">
+        <v>3892</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
       <c r="A71" s="4" t="s">
         <v>154</v>
       </c>
@@ -6371,8 +6584,11 @@
       <c r="S71">
         <v>317</v>
       </c>
-    </row>
-    <row r="72" spans="1:19">
+      <c r="T71">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
       <c r="A72" s="5" t="s">
         <v>156</v>
       </c>
@@ -6427,8 +6643,11 @@
       <c r="S72">
         <v>295</v>
       </c>
-    </row>
-    <row r="73" spans="1:19">
+      <c r="T72">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
       <c r="A73" s="4" t="s">
         <v>158</v>
       </c>
@@ -6483,8 +6702,11 @@
       <c r="S73">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:19">
+      <c r="T73">
+        <v>4279</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
       <c r="A74" s="5" t="s">
         <v>160</v>
       </c>
@@ -6539,8 +6761,11 @@
       <c r="S74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:19">
+      <c r="T74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
       <c r="A75" s="4" t="s">
         <v>162</v>
       </c>
@@ -6595,8 +6820,11 @@
       <c r="S75">
         <v>45</v>
       </c>
-    </row>
-    <row r="76" spans="1:19">
+      <c r="T75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
       <c r="A76" s="5" t="s">
         <v>164</v>
       </c>
@@ -6651,8 +6879,11 @@
       <c r="S76">
         <v>171</v>
       </c>
-    </row>
-    <row r="77" spans="1:19">
+      <c r="T76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20">
       <c r="A77" s="4" t="s">
         <v>166</v>
       </c>
@@ -6707,8 +6938,11 @@
       <c r="S77">
         <v>36</v>
       </c>
-    </row>
-    <row r="78" spans="1:19">
+      <c r="T77">
+        <v>2602</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20">
       <c r="A78" s="5" t="s">
         <v>168</v>
       </c>
@@ -6763,8 +6997,11 @@
       <c r="S78">
         <v>211</v>
       </c>
-    </row>
-    <row r="79" spans="1:19">
+      <c r="T78">
+        <v>8036</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20">
       <c r="A79" s="4" t="s">
         <v>170</v>
       </c>
@@ -6819,8 +7056,11 @@
       <c r="S79">
         <v>32</v>
       </c>
-    </row>
-    <row r="80" spans="1:19">
+      <c r="T79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20">
       <c r="A80" s="5" t="s">
         <v>172</v>
       </c>
@@ -6875,8 +7115,11 @@
       <c r="S80">
         <v>238</v>
       </c>
-    </row>
-    <row r="81" spans="1:19">
+      <c r="T80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
       <c r="A81" s="4" t="s">
         <v>174</v>
       </c>
@@ -6931,8 +7174,11 @@
       <c r="S81">
         <v>202</v>
       </c>
-    </row>
-    <row r="82" spans="1:19">
+      <c r="T81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20">
       <c r="A82" s="5" t="s">
         <v>176</v>
       </c>
@@ -6987,8 +7233,11 @@
       <c r="S82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:19">
+      <c r="T82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20">
       <c r="A83" s="4" t="s">
         <v>178</v>
       </c>
@@ -7043,8 +7292,11 @@
       <c r="S83">
         <v>309</v>
       </c>
-    </row>
-    <row r="84" spans="1:19">
+      <c r="T83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20">
       <c r="A84" s="5" t="s">
         <v>180</v>
       </c>
@@ -7099,8 +7351,11 @@
       <c r="S84">
         <v>167</v>
       </c>
-    </row>
-    <row r="85" spans="1:19">
+      <c r="T84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20">
       <c r="A85" s="4" t="s">
         <v>182</v>
       </c>
@@ -7155,8 +7410,11 @@
       <c r="S85">
         <v>308</v>
       </c>
-    </row>
-    <row r="86" spans="1:19">
+      <c r="T85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20">
       <c r="A86" s="5" t="s">
         <v>184</v>
       </c>
@@ -7211,8 +7469,11 @@
       <c r="S86">
         <v>305</v>
       </c>
-    </row>
-    <row r="87" spans="1:19">
+      <c r="T86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20">
       <c r="A87" s="4" t="s">
         <v>186</v>
       </c>
@@ -7267,8 +7528,11 @@
       <c r="S87">
         <v>267</v>
       </c>
-    </row>
-    <row r="88" spans="1:19">
+      <c r="T87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20">
       <c r="A88" s="5" t="s">
         <v>188</v>
       </c>
@@ -7323,8 +7587,11 @@
       <c r="S88">
         <v>280</v>
       </c>
-    </row>
-    <row r="89" spans="1:19">
+      <c r="T88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20">
       <c r="A89" s="4" t="s">
         <v>190</v>
       </c>
@@ -7379,8 +7646,11 @@
       <c r="S89">
         <v>290</v>
       </c>
-    </row>
-    <row r="90" spans="1:19">
+      <c r="T89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20">
       <c r="A90" s="5" t="s">
         <v>192</v>
       </c>
@@ -7435,8 +7705,11 @@
       <c r="S90">
         <v>9</v>
       </c>
-    </row>
-    <row r="91" spans="1:19">
+      <c r="T90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20">
       <c r="A91" s="4" t="s">
         <v>194</v>
       </c>
@@ -7491,8 +7764,11 @@
       <c r="S91">
         <v>283</v>
       </c>
-    </row>
-    <row r="92" spans="1:19">
+      <c r="T91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20">
       <c r="A92" s="5" t="s">
         <v>196</v>
       </c>
@@ -7544,8 +7820,11 @@
       <c r="S92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:19">
+      <c r="T92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20">
       <c r="A93" s="4" t="s">
         <v>198</v>
       </c>
@@ -7580,7 +7859,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:20">
       <c r="A94" s="6" t="s">
         <v>200</v>
       </c>
@@ -7634,6 +7913,9 @@
       </c>
       <c r="S94">
         <v>74</v>
+      </c>
+      <c r="T94">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>